<commit_message>
software pricing auto fill
</commit_message>
<xml_diff>
--- a/Country&Customer_import_upload_Model.xlsx
+++ b/Country&Customer_import_upload_Model.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crayo\Desktop\Pricing Auto\Dahua_Pricing_Auto\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AFA597-1716-468C-8036-BB971D68966D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Part No.</t>
   </si>
@@ -49,30 +43,24 @@
     <t>MSRP</t>
   </si>
   <si>
-    <t>1.0.01.04.43323-9001</t>
-  </si>
-  <si>
-    <t>1.0.01.04.43322-9001</t>
-  </si>
-  <si>
-    <t>1.0.01.04.40292-9001</t>
-  </si>
-  <si>
-    <t>1.0.01.04.43324-0005</t>
-  </si>
-  <si>
-    <t>1.0.01.04.44373-0002</t>
+    <t>1.0.01.14.12097-D001</t>
+  </si>
+  <si>
+    <t>1.0.01.14.12100</t>
+  </si>
+  <si>
+    <t>1.5.01.98.59836</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -80,21 +68,9 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,38 +108,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,7 +163,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -235,7 +197,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -270,10 +231,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -446,19 +406,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="28.375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,153 +442,58 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
-        <v>89</v>
-      </c>
-      <c r="C2" s="2">
-        <v>101</v>
-      </c>
-      <c r="D2" s="2">
-        <v>124</v>
-      </c>
-      <c r="E2" s="2">
-        <v>137</v>
-      </c>
-      <c r="F2" s="2">
-        <v>137</v>
-      </c>
-      <c r="G2" s="2">
-        <v>167</v>
-      </c>
-      <c r="H2" s="2">
-        <v>167</v>
-      </c>
-      <c r="I2" s="2">
-        <v>415</v>
+      <c r="B2">
+        <v>72</v>
+      </c>
+      <c r="C2">
+        <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
-        <v>96</v>
-      </c>
-      <c r="C3" s="2">
-        <v>112</v>
-      </c>
-      <c r="D3" s="2">
-        <v>133</v>
-      </c>
-      <c r="E3" s="2">
-        <v>146</v>
-      </c>
-      <c r="F3" s="2">
-        <v>146</v>
-      </c>
-      <c r="G3" s="2">
-        <v>180</v>
-      </c>
-      <c r="H3" s="2">
-        <v>180</v>
-      </c>
-      <c r="I3" s="2">
-        <v>444</v>
+      <c r="B3">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2">
-        <v>60</v>
-      </c>
-      <c r="C4" s="2">
-        <v>68</v>
-      </c>
-      <c r="D4" s="2">
-        <v>80</v>
-      </c>
-      <c r="E4" s="2">
-        <v>93</v>
-      </c>
-      <c r="F4" s="2">
-        <v>93</v>
-      </c>
-      <c r="G4" s="2">
-        <v>107</v>
-      </c>
-      <c r="H4" s="2">
-        <v>107</v>
-      </c>
-      <c r="I4" s="2">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2">
-        <v>131</v>
-      </c>
-      <c r="C5" s="2">
-        <v>149</v>
-      </c>
-      <c r="D5" s="2">
-        <v>183</v>
-      </c>
-      <c r="E5" s="2">
-        <v>201</v>
-      </c>
-      <c r="F5" s="2">
-        <v>201</v>
-      </c>
-      <c r="G5" s="2">
-        <v>247</v>
-      </c>
-      <c r="H5" s="2">
-        <v>247</v>
-      </c>
-      <c r="I5" s="2">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2">
-        <v>59</v>
-      </c>
-      <c r="C6" s="2">
-        <v>66</v>
-      </c>
-      <c r="D6" s="2">
-        <v>75</v>
-      </c>
-      <c r="E6" s="2">
-        <v>84</v>
-      </c>
-      <c r="F6" s="2">
-        <v>84</v>
-      </c>
-      <c r="G6" s="2">
-        <v>101</v>
-      </c>
-      <c r="H6" s="2">
-        <v>101</v>
-      </c>
-      <c r="I6" s="2">
-        <v>249</v>
+      <c r="B4">
+        <v>1616</v>
+      </c>
+      <c r="C4">
+        <v>1876</v>
+      </c>
+      <c r="D4">
+        <v>2207</v>
+      </c>
+      <c r="E4">
+        <v>2501</v>
+      </c>
+      <c r="F4">
+        <v>2501</v>
+      </c>
+      <c r="G4">
+        <v>2679</v>
+      </c>
+      <c r="H4">
+        <v>2886</v>
+      </c>
+      <c r="I4">
+        <v>4809</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>